<commit_message>
add population of Transport Order List
</commit_message>
<xml_diff>
--- a/Data/Example_DataSet.xlsx
+++ b/Data/Example_DataSet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucas\Google Drive\Career\Education\Beuth Data Science\LearningOptimization\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucas\Google Drive\Career\Education\Beuth Data Science\LearningOptimization\Project\MilkRunOptimizer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7312CD94-8D76-489F-A8B3-8A3E94EFB1B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47D5DE2A-5256-4ADE-BAD2-822783A7986F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10620" yWindow="3060" windowWidth="21600" windowHeight="11505" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-30" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Visualization" sheetId="6" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="283">
   <si>
     <t>Planning Status</t>
   </si>
@@ -861,6 +861,21 @@
   </si>
   <si>
     <t>Nuremburg-&gt;Stuttgart</t>
+  </si>
+  <si>
+    <t>Nuremburg</t>
+  </si>
+  <si>
+    <t>Munich</t>
+  </si>
+  <si>
+    <t>Stuttgart</t>
+  </si>
+  <si>
+    <t>Supplier S.A (Porto)</t>
+  </si>
+  <si>
+    <t>Supplier Lda (Barcelona)</t>
   </si>
 </sst>
 </file>
@@ -1457,10 +1472,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:Q46"/>
+  <dimension ref="A1:T46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1477,7 +1492,7 @@
     <col min="15" max="15" width="20.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>160</v>
       </c>
@@ -1503,7 +1518,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1544,7 +1559,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1585,7 +1600,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1626,7 +1641,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1658,7 +1673,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -1690,7 +1705,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -1722,7 +1737,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -1754,7 +1769,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1785,8 +1800,14 @@
       <c r="J10" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="O10" t="s">
+        <v>278</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1817,8 +1838,17 @@
       <c r="J11" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="O11" t="s">
+        <v>279</v>
+      </c>
+      <c r="P11">
+        <v>170</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1849,8 +1879,20 @@
       <c r="J12" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="O12" t="s">
+        <v>280</v>
+      </c>
+      <c r="P12">
+        <v>210</v>
+      </c>
+      <c r="Q12">
+        <v>243</v>
+      </c>
+      <c r="R12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -1881,8 +1923,23 @@
       <c r="J13" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="O13" t="s">
+        <v>281</v>
+      </c>
+      <c r="P13">
+        <v>2219</v>
+      </c>
+      <c r="Q13">
+        <v>2253</v>
+      </c>
+      <c r="R13">
+        <v>2042</v>
+      </c>
+      <c r="S13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -1913,8 +1970,26 @@
       <c r="J14" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="O14" t="s">
+        <v>282</v>
+      </c>
+      <c r="P14">
+        <v>1444</v>
+      </c>
+      <c r="Q14">
+        <v>1369</v>
+      </c>
+      <c r="R14">
+        <v>1267</v>
+      </c>
+      <c r="S14">
+        <v>1127</v>
+      </c>
+      <c r="T14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -1946,7 +2021,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
Started implementing OR Tools
</commit_message>
<xml_diff>
--- a/Data/Example_DataSet.xlsx
+++ b/Data/Example_DataSet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucas\Google Drive\Career\Education\Beuth Data Science\LearningOptimization\Project\MilkRunOptimizer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47D5DE2A-5256-4ADE-BAD2-822783A7986F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48564A3C-1D04-41C4-99B9-81B57F3B75CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-30" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24870" yWindow="2280" windowWidth="21600" windowHeight="11505" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Visualization" sheetId="6" r:id="rId1"/>
@@ -1474,8 +1474,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:T46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="P15" sqref="P15"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10:N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1800,6 +1800,9 @@
       <c r="J10" t="s">
         <v>44</v>
       </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
       <c r="O10" t="s">
         <v>278</v>
       </c>
@@ -1838,6 +1841,9 @@
       <c r="J11" t="s">
         <v>48</v>
       </c>
+      <c r="N11">
+        <v>1</v>
+      </c>
       <c r="O11" t="s">
         <v>279</v>
       </c>
@@ -1879,6 +1885,9 @@
       <c r="J12" t="s">
         <v>52</v>
       </c>
+      <c r="N12">
+        <v>2</v>
+      </c>
       <c r="O12" t="s">
         <v>280</v>
       </c>
@@ -1923,6 +1932,9 @@
       <c r="J13" t="s">
         <v>56</v>
       </c>
+      <c r="N13" s="6">
+        <v>3</v>
+      </c>
       <c r="O13" t="s">
         <v>281</v>
       </c>
@@ -1969,6 +1981,9 @@
       </c>
       <c r="J14" t="s">
         <v>60</v>
+      </c>
+      <c r="N14" s="6">
+        <v>4</v>
       </c>
       <c r="O14" t="s">
         <v>282</v>

</xml_diff>